<commit_message>
add error message when user click button
</commit_message>
<xml_diff>
--- a/excel/barcode.xlsx
+++ b/excel/barcode.xlsx
@@ -16,304 +16,304 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
-    <t>223-wwe-223</t>
-  </si>
-  <si>
-    <t>223-wwe-224</t>
-  </si>
-  <si>
-    <t>223-wwe-225</t>
-  </si>
-  <si>
-    <t>223-wwe-226</t>
-  </si>
-  <si>
-    <t>223-wwe-227</t>
-  </si>
-  <si>
-    <t>223-wwe-228</t>
-  </si>
-  <si>
-    <t>223-wwe-229</t>
-  </si>
-  <si>
-    <t>223-wwe-230</t>
-  </si>
-  <si>
-    <t>223-wwe-231</t>
-  </si>
-  <si>
-    <t>223-wwe-232</t>
-  </si>
-  <si>
-    <t>223-wwe-233</t>
-  </si>
-  <si>
-    <t>223-wwe-234</t>
-  </si>
-  <si>
-    <t>223-wwe-235</t>
-  </si>
-  <si>
-    <t>223-wwe-236</t>
-  </si>
-  <si>
-    <t>223-wwe-237</t>
-  </si>
-  <si>
-    <t>223-wwe-238</t>
-  </si>
-  <si>
-    <t>223-wwe-239</t>
-  </si>
-  <si>
-    <t>223-wwe-240</t>
-  </si>
-  <si>
-    <t>223-wwe-241</t>
-  </si>
-  <si>
-    <t>223-wwe-242</t>
-  </si>
-  <si>
-    <t>223-wwe-243</t>
-  </si>
-  <si>
-    <t>223-wwe-244</t>
-  </si>
-  <si>
-    <t>223-wwe-245</t>
-  </si>
-  <si>
-    <t>223-wwe-246</t>
-  </si>
-  <si>
-    <t>223-wwe-247</t>
-  </si>
-  <si>
-    <t>223-wwe-248</t>
-  </si>
-  <si>
-    <t>223-wwe-249</t>
-  </si>
-  <si>
-    <t>223-wwe-250</t>
-  </si>
-  <si>
-    <t>223-wwe-251</t>
-  </si>
-  <si>
-    <t>223-wwe-252</t>
-  </si>
-  <si>
-    <t>223-wwe-253</t>
-  </si>
-  <si>
-    <t>223-wwe-254</t>
-  </si>
-  <si>
-    <t>223-wwe-255</t>
-  </si>
-  <si>
-    <t>223-wwe-256</t>
-  </si>
-  <si>
-    <t>223-wwe-257</t>
-  </si>
-  <si>
-    <t>223-wwe-258</t>
-  </si>
-  <si>
-    <t>223-wwe-259</t>
-  </si>
-  <si>
-    <t>223-wwe-260</t>
-  </si>
-  <si>
-    <t>223-wwe-261</t>
-  </si>
-  <si>
-    <t>223-wwe-262</t>
-  </si>
-  <si>
-    <t>223-wwe-263</t>
-  </si>
-  <si>
-    <t>223-wwe-264</t>
-  </si>
-  <si>
-    <t>223-wwe-265</t>
-  </si>
-  <si>
-    <t>223-wwe-266</t>
-  </si>
-  <si>
-    <t>223-wwe-267</t>
-  </si>
-  <si>
-    <t>223-wwe-268</t>
-  </si>
-  <si>
-    <t>223-wwe-269</t>
-  </si>
-  <si>
-    <t>223-wwe-270</t>
-  </si>
-  <si>
-    <t>223-wwe-271</t>
-  </si>
-  <si>
-    <t>223-wwe-272</t>
-  </si>
-  <si>
-    <t>223-wwe-273</t>
-  </si>
-  <si>
-    <t>223-wwe-274</t>
-  </si>
-  <si>
-    <t>223-wwe-275</t>
-  </si>
-  <si>
-    <t>223-wwe-276</t>
-  </si>
-  <si>
-    <t>223-wwe-277</t>
-  </si>
-  <si>
-    <t>223-wwe-278</t>
-  </si>
-  <si>
-    <t>223-wwe-279</t>
-  </si>
-  <si>
-    <t>223-wwe-280</t>
-  </si>
-  <si>
-    <t>223-wwe-281</t>
-  </si>
-  <si>
-    <t>223-wwe-282</t>
-  </si>
-  <si>
-    <t>223-wwe-283</t>
-  </si>
-  <si>
-    <t>223-wwe-284</t>
-  </si>
-  <si>
-    <t>223-wwe-285</t>
-  </si>
-  <si>
-    <t>223-wwe-286</t>
-  </si>
-  <si>
-    <t>223-wwe-287</t>
-  </si>
-  <si>
-    <t>223-wwe-288</t>
-  </si>
-  <si>
-    <t>223-wwe-289</t>
-  </si>
-  <si>
-    <t>223-wwe-290</t>
-  </si>
-  <si>
-    <t>223-wwe-291</t>
-  </si>
-  <si>
-    <t>223-wwe-292</t>
-  </si>
-  <si>
-    <t>223-wwe-293</t>
-  </si>
-  <si>
-    <t>223-wwe-294</t>
-  </si>
-  <si>
-    <t>223-wwe-295</t>
-  </si>
-  <si>
-    <t>223-wwe-296</t>
-  </si>
-  <si>
-    <t>223-wwe-297</t>
-  </si>
-  <si>
-    <t>223-wwe-298</t>
-  </si>
-  <si>
-    <t>223-wwe-299</t>
-  </si>
-  <si>
-    <t>223-wwe-300</t>
-  </si>
-  <si>
-    <t>223-wwe-301</t>
-  </si>
-  <si>
-    <t>223-wwe-302</t>
-  </si>
-  <si>
-    <t>223-wwe-303</t>
-  </si>
-  <si>
-    <t>223-wwe-304</t>
-  </si>
-  <si>
-    <t>223-wwe-305</t>
-  </si>
-  <si>
-    <t>223-wwe-306</t>
-  </si>
-  <si>
-    <t>223-wwe-307</t>
-  </si>
-  <si>
-    <t>223-wwe-308</t>
-  </si>
-  <si>
-    <t>223-wwe-309</t>
-  </si>
-  <si>
-    <t>223-wwe-310</t>
-  </si>
-  <si>
-    <t>223-wwe-311</t>
-  </si>
-  <si>
-    <t>223-wwe-312</t>
-  </si>
-  <si>
-    <t>223-wwe-313</t>
-  </si>
-  <si>
-    <t>223-wwe-314</t>
-  </si>
-  <si>
-    <t>223-wwe-315</t>
-  </si>
-  <si>
-    <t>223-wwe-316</t>
-  </si>
-  <si>
-    <t>223-wwe-317</t>
-  </si>
-  <si>
-    <t>223-wwe-318</t>
-  </si>
-  <si>
-    <t>223-wwe-319</t>
-  </si>
-  <si>
-    <t>223-wwe-320</t>
-  </si>
-  <si>
-    <t>223-wwe-321</t>
-  </si>
-  <si>
-    <t>223-wwe-322</t>
+    <t>RM-100</t>
+  </si>
+  <si>
+    <t>RM-101</t>
+  </si>
+  <si>
+    <t>RM-102</t>
+  </si>
+  <si>
+    <t>RM-103</t>
+  </si>
+  <si>
+    <t>RM-104</t>
+  </si>
+  <si>
+    <t>RM-105</t>
+  </si>
+  <si>
+    <t>RM-106</t>
+  </si>
+  <si>
+    <t>RM-107</t>
+  </si>
+  <si>
+    <t>RM-108</t>
+  </si>
+  <si>
+    <t>RM-109</t>
+  </si>
+  <si>
+    <t>RM-110</t>
+  </si>
+  <si>
+    <t>RM-111</t>
+  </si>
+  <si>
+    <t>RM-112</t>
+  </si>
+  <si>
+    <t>RM-113</t>
+  </si>
+  <si>
+    <t>RM-114</t>
+  </si>
+  <si>
+    <t>RM-115</t>
+  </si>
+  <si>
+    <t>RM-116</t>
+  </si>
+  <si>
+    <t>RM-117</t>
+  </si>
+  <si>
+    <t>RM-118</t>
+  </si>
+  <si>
+    <t>RM-119</t>
+  </si>
+  <si>
+    <t>RM-120</t>
+  </si>
+  <si>
+    <t>RM-121</t>
+  </si>
+  <si>
+    <t>RM-122</t>
+  </si>
+  <si>
+    <t>RM-123</t>
+  </si>
+  <si>
+    <t>RM-124</t>
+  </si>
+  <si>
+    <t>RM-125</t>
+  </si>
+  <si>
+    <t>RM-126</t>
+  </si>
+  <si>
+    <t>RM-127</t>
+  </si>
+  <si>
+    <t>RM-128</t>
+  </si>
+  <si>
+    <t>RM-129</t>
+  </si>
+  <si>
+    <t>RM-130</t>
+  </si>
+  <si>
+    <t>RM-131</t>
+  </si>
+  <si>
+    <t>RM-132</t>
+  </si>
+  <si>
+    <t>RM-133</t>
+  </si>
+  <si>
+    <t>RM-134</t>
+  </si>
+  <si>
+    <t>RM-135</t>
+  </si>
+  <si>
+    <t>RM-136</t>
+  </si>
+  <si>
+    <t>RM-137</t>
+  </si>
+  <si>
+    <t>RM-138</t>
+  </si>
+  <si>
+    <t>RM-139</t>
+  </si>
+  <si>
+    <t>RM-140</t>
+  </si>
+  <si>
+    <t>RM-141</t>
+  </si>
+  <si>
+    <t>RM-142</t>
+  </si>
+  <si>
+    <t>RM-143</t>
+  </si>
+  <si>
+    <t>RM-144</t>
+  </si>
+  <si>
+    <t>RM-145</t>
+  </si>
+  <si>
+    <t>RM-146</t>
+  </si>
+  <si>
+    <t>RM-147</t>
+  </si>
+  <si>
+    <t>RM-148</t>
+  </si>
+  <si>
+    <t>RM-149</t>
+  </si>
+  <si>
+    <t>RM-150</t>
+  </si>
+  <si>
+    <t>RM-151</t>
+  </si>
+  <si>
+    <t>RM-152</t>
+  </si>
+  <si>
+    <t>RM-153</t>
+  </si>
+  <si>
+    <t>RM-154</t>
+  </si>
+  <si>
+    <t>RM-155</t>
+  </si>
+  <si>
+    <t>RM-156</t>
+  </si>
+  <si>
+    <t>RM-157</t>
+  </si>
+  <si>
+    <t>RM-158</t>
+  </si>
+  <si>
+    <t>RM-159</t>
+  </si>
+  <si>
+    <t>RM-160</t>
+  </si>
+  <si>
+    <t>RM-161</t>
+  </si>
+  <si>
+    <t>RM-162</t>
+  </si>
+  <si>
+    <t>RM-163</t>
+  </si>
+  <si>
+    <t>RM-164</t>
+  </si>
+  <si>
+    <t>RM-165</t>
+  </si>
+  <si>
+    <t>RM-166</t>
+  </si>
+  <si>
+    <t>RM-167</t>
+  </si>
+  <si>
+    <t>RM-168</t>
+  </si>
+  <si>
+    <t>RM-169</t>
+  </si>
+  <si>
+    <t>RM-170</t>
+  </si>
+  <si>
+    <t>RM-171</t>
+  </si>
+  <si>
+    <t>RM-172</t>
+  </si>
+  <si>
+    <t>RM-173</t>
+  </si>
+  <si>
+    <t>RM-174</t>
+  </si>
+  <si>
+    <t>RM-175</t>
+  </si>
+  <si>
+    <t>RM-176</t>
+  </si>
+  <si>
+    <t>RM-177</t>
+  </si>
+  <si>
+    <t>RM-178</t>
+  </si>
+  <si>
+    <t>RM-179</t>
+  </si>
+  <si>
+    <t>RM-180</t>
+  </si>
+  <si>
+    <t>RM-181</t>
+  </si>
+  <si>
+    <t>RM-182</t>
+  </si>
+  <si>
+    <t>RM-183</t>
+  </si>
+  <si>
+    <t>RM-184</t>
+  </si>
+  <si>
+    <t>RM-185</t>
+  </si>
+  <si>
+    <t>RM-186</t>
+  </si>
+  <si>
+    <t>RM-187</t>
+  </si>
+  <si>
+    <t>RM-188</t>
+  </si>
+  <si>
+    <t>RM-189</t>
+  </si>
+  <si>
+    <t>RM-190</t>
+  </si>
+  <si>
+    <t>RM-191</t>
+  </si>
+  <si>
+    <t>RM-192</t>
+  </si>
+  <si>
+    <t>RM-193</t>
+  </si>
+  <si>
+    <t>RM-194</t>
+  </si>
+  <si>
+    <t>RM-195</t>
+  </si>
+  <si>
+    <t>RM-196</t>
+  </si>
+  <si>
+    <t>RM-197</t>
+  </si>
+  <si>
+    <t>RM-198</t>
+  </si>
+  <si>
+    <t>RM-199</t>
   </si>
 </sst>
 </file>
@@ -373,14 +373,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="223-wwe-223.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="RM-100.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -394,7 +394,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="0"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -411,14 +411,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="223-wwe-224.png"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="RM-101.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -432,7 +432,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="1009650"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -449,14 +449,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="223-wwe-225.png"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="RM-102.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -470,7 +470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="2019300"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -487,14 +487,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="223-wwe-226.png"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="RM-103.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -508,7 +508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="3028950"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -525,14 +525,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="223-wwe-227.png"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="RM-104.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -546,7 +546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="4038600"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -563,14 +563,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="223-wwe-228.png"/>
+        <xdr:cNvPr id="7" name="Picture 6" descr="RM-105.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -584,7 +584,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="5048250"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -601,14 +601,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="223-wwe-229.png"/>
+        <xdr:cNvPr id="8" name="Picture 7" descr="RM-106.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -622,7 +622,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="6057900"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -639,14 +639,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="223-wwe-230.png"/>
+        <xdr:cNvPr id="9" name="Picture 8" descr="RM-107.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -660,7 +660,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="7067550"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -677,14 +677,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="223-wwe-231.png"/>
+        <xdr:cNvPr id="10" name="Picture 9" descr="RM-108.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -698,7 +698,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="8077200"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -715,14 +715,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="223-wwe-232.png"/>
+        <xdr:cNvPr id="11" name="Picture 10" descr="RM-109.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -736,7 +736,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="9086850"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -753,14 +753,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="223-wwe-233.png"/>
+        <xdr:cNvPr id="12" name="Picture 11" descr="RM-110.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -774,7 +774,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="10096500"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -791,14 +791,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="223-wwe-234.png"/>
+        <xdr:cNvPr id="13" name="Picture 12" descr="RM-111.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -812,7 +812,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="11106150"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -829,14 +829,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="223-wwe-235.png"/>
+        <xdr:cNvPr id="14" name="Picture 13" descr="RM-112.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -850,7 +850,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="12115800"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -867,14 +867,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14" descr="223-wwe-236.png"/>
+        <xdr:cNvPr id="15" name="Picture 14" descr="RM-113.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -888,7 +888,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="13125450"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -905,14 +905,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15" descr="223-wwe-237.png"/>
+        <xdr:cNvPr id="16" name="Picture 15" descr="RM-114.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -926,7 +926,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="14135100"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -943,14 +943,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16" descr="223-wwe-238.png"/>
+        <xdr:cNvPr id="17" name="Picture 16" descr="RM-115.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -964,7 +964,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="15144750"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -981,14 +981,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17" descr="223-wwe-239.png"/>
+        <xdr:cNvPr id="18" name="Picture 17" descr="RM-116.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1002,7 +1002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="16154400"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1019,14 +1019,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18" descr="223-wwe-240.png"/>
+        <xdr:cNvPr id="19" name="Picture 18" descr="RM-117.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1040,7 +1040,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="17164050"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1057,14 +1057,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19" descr="223-wwe-241.png"/>
+        <xdr:cNvPr id="20" name="Picture 19" descr="RM-118.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1078,7 +1078,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="18173700"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1095,14 +1095,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20" descr="223-wwe-242.png"/>
+        <xdr:cNvPr id="21" name="Picture 20" descr="RM-119.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1116,7 +1116,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="19183350"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1133,14 +1133,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21" descr="223-wwe-243.png"/>
+        <xdr:cNvPr id="22" name="Picture 21" descr="RM-120.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1154,7 +1154,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="20193000"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1171,14 +1171,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22" descr="223-wwe-244.png"/>
+        <xdr:cNvPr id="23" name="Picture 22" descr="RM-121.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1192,7 +1192,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="21202650"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1209,14 +1209,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23" descr="223-wwe-245.png"/>
+        <xdr:cNvPr id="24" name="Picture 23" descr="RM-122.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1230,7 +1230,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="22212300"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1247,14 +1247,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24" descr="223-wwe-246.png"/>
+        <xdr:cNvPr id="25" name="Picture 24" descr="RM-123.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1268,7 +1268,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="23221950"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1285,14 +1285,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 25" descr="223-wwe-247.png"/>
+        <xdr:cNvPr id="26" name="Picture 25" descr="RM-124.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1306,7 +1306,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="24231600"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1323,14 +1323,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 26" descr="223-wwe-248.png"/>
+        <xdr:cNvPr id="27" name="Picture 26" descr="RM-125.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1344,7 +1344,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="25241250"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1361,14 +1361,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Picture 27" descr="223-wwe-249.png"/>
+        <xdr:cNvPr id="28" name="Picture 27" descr="RM-126.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1382,7 +1382,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="26250900"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1399,14 +1399,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Picture 28" descr="223-wwe-250.png"/>
+        <xdr:cNvPr id="29" name="Picture 28" descr="RM-127.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1420,7 +1420,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="27260550"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1437,14 +1437,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Picture 29" descr="223-wwe-251.png"/>
+        <xdr:cNvPr id="30" name="Picture 29" descr="RM-128.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1458,7 +1458,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="28270200"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1475,14 +1475,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Picture 30" descr="223-wwe-252.png"/>
+        <xdr:cNvPr id="31" name="Picture 30" descr="RM-129.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1496,7 +1496,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="29279850"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1513,14 +1513,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Picture 31" descr="223-wwe-253.png"/>
+        <xdr:cNvPr id="32" name="Picture 31" descr="RM-130.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1534,7 +1534,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="30289500"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1551,14 +1551,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Picture 32" descr="223-wwe-254.png"/>
+        <xdr:cNvPr id="33" name="Picture 32" descr="RM-131.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1572,7 +1572,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="31299150"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1589,14 +1589,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Picture 33" descr="223-wwe-255.png"/>
+        <xdr:cNvPr id="34" name="Picture 33" descr="RM-132.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1610,7 +1610,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="32308800"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1627,14 +1627,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Picture 34" descr="223-wwe-256.png"/>
+        <xdr:cNvPr id="35" name="Picture 34" descr="RM-133.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1648,7 +1648,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="33318450"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1665,14 +1665,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="Picture 35" descr="223-wwe-257.png"/>
+        <xdr:cNvPr id="36" name="Picture 35" descr="RM-134.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1686,7 +1686,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="34328100"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1703,14 +1703,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Picture 36" descr="223-wwe-258.png"/>
+        <xdr:cNvPr id="37" name="Picture 36" descr="RM-135.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1724,7 +1724,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="35337750"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1741,14 +1741,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 37" descr="223-wwe-259.png"/>
+        <xdr:cNvPr id="38" name="Picture 37" descr="RM-136.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1762,7 +1762,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="36347400"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1779,14 +1779,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Picture 38" descr="223-wwe-260.png"/>
+        <xdr:cNvPr id="39" name="Picture 38" descr="RM-137.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1800,7 +1800,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="37357050"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1817,14 +1817,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="Picture 39" descr="223-wwe-261.png"/>
+        <xdr:cNvPr id="40" name="Picture 39" descr="RM-138.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1838,7 +1838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="38366700"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1855,14 +1855,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Picture 40" descr="223-wwe-262.png"/>
+        <xdr:cNvPr id="41" name="Picture 40" descr="RM-139.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1876,7 +1876,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="39376350"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1893,14 +1893,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="Picture 41" descr="223-wwe-263.png"/>
+        <xdr:cNvPr id="42" name="Picture 41" descr="RM-140.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1914,7 +1914,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="40386000"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1931,14 +1931,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="Picture 42" descr="223-wwe-264.png"/>
+        <xdr:cNvPr id="43" name="Picture 42" descr="RM-141.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1952,7 +1952,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="41395650"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1969,14 +1969,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="44" name="Picture 43" descr="223-wwe-265.png"/>
+        <xdr:cNvPr id="44" name="Picture 43" descr="RM-142.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1990,7 +1990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="42405300"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2007,14 +2007,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="45" name="Picture 44" descr="223-wwe-266.png"/>
+        <xdr:cNvPr id="45" name="Picture 44" descr="RM-143.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2028,7 +2028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="43414950"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2045,14 +2045,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="46" name="Picture 45" descr="223-wwe-267.png"/>
+        <xdr:cNvPr id="46" name="Picture 45" descr="RM-144.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2066,7 +2066,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="44424600"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2083,14 +2083,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="Picture 46" descr="223-wwe-268.png"/>
+        <xdr:cNvPr id="47" name="Picture 46" descr="RM-145.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2104,7 +2104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="45434250"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2121,14 +2121,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="48" name="Picture 47" descr="223-wwe-269.png"/>
+        <xdr:cNvPr id="48" name="Picture 47" descr="RM-146.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2142,7 +2142,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="46443900"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2159,14 +2159,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="49" name="Picture 48" descr="223-wwe-270.png"/>
+        <xdr:cNvPr id="49" name="Picture 48" descr="RM-147.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2180,7 +2180,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="47453550"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2197,14 +2197,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="50" name="Picture 49" descr="223-wwe-271.png"/>
+        <xdr:cNvPr id="50" name="Picture 49" descr="RM-148.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2218,7 +2218,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="48463200"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2235,14 +2235,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="51" name="Picture 50" descr="223-wwe-272.png"/>
+        <xdr:cNvPr id="51" name="Picture 50" descr="RM-149.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2256,7 +2256,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="49472850"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2273,14 +2273,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="52" name="Picture 51" descr="223-wwe-273.png"/>
+        <xdr:cNvPr id="52" name="Picture 51" descr="RM-150.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2294,7 +2294,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="50482500"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2311,14 +2311,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="53" name="Picture 52" descr="223-wwe-274.png"/>
+        <xdr:cNvPr id="53" name="Picture 52" descr="RM-151.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2332,7 +2332,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="51492150"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2349,14 +2349,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="54" name="Picture 53" descr="223-wwe-275.png"/>
+        <xdr:cNvPr id="54" name="Picture 53" descr="RM-152.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2370,7 +2370,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="52501800"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2387,14 +2387,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="Picture 54" descr="223-wwe-276.png"/>
+        <xdr:cNvPr id="55" name="Picture 54" descr="RM-153.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2408,7 +2408,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="53511450"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2425,14 +2425,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="56" name="Picture 55" descr="223-wwe-277.png"/>
+        <xdr:cNvPr id="56" name="Picture 55" descr="RM-154.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2446,7 +2446,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="54521100"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2463,14 +2463,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="57" name="Picture 56" descr="223-wwe-278.png"/>
+        <xdr:cNvPr id="57" name="Picture 56" descr="RM-155.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2484,7 +2484,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="55530750"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2501,14 +2501,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="58" name="Picture 57" descr="223-wwe-279.png"/>
+        <xdr:cNvPr id="58" name="Picture 57" descr="RM-156.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2522,7 +2522,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="56540400"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2539,14 +2539,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="59" name="Picture 58" descr="223-wwe-280.png"/>
+        <xdr:cNvPr id="59" name="Picture 58" descr="RM-157.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2560,7 +2560,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="57550050"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2577,14 +2577,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="60" name="Picture 59" descr="223-wwe-281.png"/>
+        <xdr:cNvPr id="60" name="Picture 59" descr="RM-158.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2598,7 +2598,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="58559700"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2615,14 +2615,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61" name="Picture 60" descr="223-wwe-282.png"/>
+        <xdr:cNvPr id="61" name="Picture 60" descr="RM-159.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2636,7 +2636,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="59569350"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2653,14 +2653,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="62" name="Picture 61" descr="223-wwe-283.png"/>
+        <xdr:cNvPr id="62" name="Picture 61" descr="RM-160.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2674,7 +2674,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="60579000"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2691,14 +2691,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="63" name="Picture 62" descr="223-wwe-284.png"/>
+        <xdr:cNvPr id="63" name="Picture 62" descr="RM-161.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2712,7 +2712,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="61588650"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2729,14 +2729,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="64" name="Picture 63" descr="223-wwe-285.png"/>
+        <xdr:cNvPr id="64" name="Picture 63" descr="RM-162.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2750,7 +2750,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="62598300"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2767,14 +2767,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="65" name="Picture 64" descr="223-wwe-286.png"/>
+        <xdr:cNvPr id="65" name="Picture 64" descr="RM-163.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2788,7 +2788,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="63607950"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2805,14 +2805,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="66" name="Picture 65" descr="223-wwe-287.png"/>
+        <xdr:cNvPr id="66" name="Picture 65" descr="RM-164.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2826,7 +2826,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="64617600"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2843,14 +2843,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="67" name="Picture 66" descr="223-wwe-288.png"/>
+        <xdr:cNvPr id="67" name="Picture 66" descr="RM-165.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2864,7 +2864,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="65627250"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2881,14 +2881,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="68" name="Picture 67" descr="223-wwe-289.png"/>
+        <xdr:cNvPr id="68" name="Picture 67" descr="RM-166.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2902,7 +2902,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="66636900"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2919,14 +2919,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="69" name="Picture 68" descr="223-wwe-290.png"/>
+        <xdr:cNvPr id="69" name="Picture 68" descr="RM-167.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2940,7 +2940,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="67646550"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2957,14 +2957,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="Picture 69" descr="223-wwe-291.png"/>
+        <xdr:cNvPr id="70" name="Picture 69" descr="RM-168.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2978,7 +2978,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="68656200"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2995,14 +2995,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="71" name="Picture 70" descr="223-wwe-292.png"/>
+        <xdr:cNvPr id="71" name="Picture 70" descr="RM-169.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3016,7 +3016,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="69665850"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3033,14 +3033,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="72" name="Picture 71" descr="223-wwe-293.png"/>
+        <xdr:cNvPr id="72" name="Picture 71" descr="RM-170.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3054,7 +3054,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="70675500"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3071,14 +3071,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="73" name="Picture 72" descr="223-wwe-294.png"/>
+        <xdr:cNvPr id="73" name="Picture 72" descr="RM-171.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3092,7 +3092,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="71685150"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3109,14 +3109,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="74" name="Picture 73" descr="223-wwe-295.png"/>
+        <xdr:cNvPr id="74" name="Picture 73" descr="RM-172.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3130,7 +3130,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="72694800"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3147,14 +3147,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="75" name="Picture 74" descr="223-wwe-296.png"/>
+        <xdr:cNvPr id="75" name="Picture 74" descr="RM-173.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3168,7 +3168,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="73704450"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3185,14 +3185,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="76" name="Picture 75" descr="223-wwe-297.png"/>
+        <xdr:cNvPr id="76" name="Picture 75" descr="RM-174.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3206,7 +3206,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="74714100"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3223,14 +3223,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="77" name="Picture 76" descr="223-wwe-298.png"/>
+        <xdr:cNvPr id="77" name="Picture 76" descr="RM-175.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3244,7 +3244,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="75723750"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3261,14 +3261,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="78" name="Picture 77" descr="223-wwe-299.png"/>
+        <xdr:cNvPr id="78" name="Picture 77" descr="RM-176.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3282,7 +3282,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="76733400"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3299,14 +3299,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>77</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="79" name="Picture 78" descr="223-wwe-300.png"/>
+        <xdr:cNvPr id="79" name="Picture 78" descr="RM-177.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3320,7 +3320,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="77743050"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3337,14 +3337,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="80" name="Picture 79" descr="223-wwe-301.png"/>
+        <xdr:cNvPr id="80" name="Picture 79" descr="RM-178.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3358,7 +3358,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="78752700"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3375,14 +3375,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="81" name="Picture 80" descr="223-wwe-302.png"/>
+        <xdr:cNvPr id="81" name="Picture 80" descr="RM-179.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3396,7 +3396,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="79762350"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3413,14 +3413,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>80</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="82" name="Picture 81" descr="223-wwe-303.png"/>
+        <xdr:cNvPr id="82" name="Picture 81" descr="RM-180.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3434,7 +3434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="80772000"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3451,14 +3451,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="83" name="Picture 82" descr="223-wwe-304.png"/>
+        <xdr:cNvPr id="83" name="Picture 82" descr="RM-181.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3472,7 +3472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="81781650"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3489,14 +3489,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="84" name="Picture 83" descr="223-wwe-305.png"/>
+        <xdr:cNvPr id="84" name="Picture 83" descr="RM-182.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3510,7 +3510,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="82791300"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3527,14 +3527,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="85" name="Picture 84" descr="223-wwe-306.png"/>
+        <xdr:cNvPr id="85" name="Picture 84" descr="RM-183.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3548,7 +3548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="83800950"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3565,14 +3565,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="86" name="Picture 85" descr="223-wwe-307.png"/>
+        <xdr:cNvPr id="86" name="Picture 85" descr="RM-184.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3586,7 +3586,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="84810600"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3603,14 +3603,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="87" name="Picture 86" descr="223-wwe-308.png"/>
+        <xdr:cNvPr id="87" name="Picture 86" descr="RM-185.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3624,7 +3624,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="85820250"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3641,14 +3641,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>86</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="88" name="Picture 87" descr="223-wwe-309.png"/>
+        <xdr:cNvPr id="88" name="Picture 87" descr="RM-186.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3662,7 +3662,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="86829900"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3679,14 +3679,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>87</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="89" name="Picture 88" descr="223-wwe-310.png"/>
+        <xdr:cNvPr id="89" name="Picture 88" descr="RM-187.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3700,7 +3700,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="87839550"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3717,14 +3717,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="90" name="Picture 89" descr="223-wwe-311.png"/>
+        <xdr:cNvPr id="90" name="Picture 89" descr="RM-188.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3738,7 +3738,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="88849200"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3755,14 +3755,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>89</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="91" name="Picture 90" descr="223-wwe-312.png"/>
+        <xdr:cNvPr id="91" name="Picture 90" descr="RM-189.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3776,7 +3776,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="89858850"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3793,14 +3793,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>90</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="92" name="Picture 91" descr="223-wwe-313.png"/>
+        <xdr:cNvPr id="92" name="Picture 91" descr="RM-190.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3814,7 +3814,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="90868500"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3831,14 +3831,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>91</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="93" name="Picture 92" descr="223-wwe-314.png"/>
+        <xdr:cNvPr id="93" name="Picture 92" descr="RM-191.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3852,7 +3852,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="91878150"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3869,14 +3869,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>92</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="94" name="Picture 93" descr="223-wwe-315.png"/>
+        <xdr:cNvPr id="94" name="Picture 93" descr="RM-192.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3890,7 +3890,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="92887800"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3907,14 +3907,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="95" name="Picture 94" descr="223-wwe-316.png"/>
+        <xdr:cNvPr id="95" name="Picture 94" descr="RM-193.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3928,7 +3928,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="93897450"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3945,14 +3945,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>94</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="96" name="Picture 95" descr="223-wwe-317.png"/>
+        <xdr:cNvPr id="96" name="Picture 95" descr="RM-194.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3966,7 +3966,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="94907100"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3983,14 +3983,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="97" name="Picture 96" descr="223-wwe-318.png"/>
+        <xdr:cNvPr id="97" name="Picture 96" descr="RM-195.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4004,7 +4004,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="95916750"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4021,14 +4021,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>96</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="98" name="Picture 97" descr="223-wwe-319.png"/>
+        <xdr:cNvPr id="98" name="Picture 97" descr="RM-196.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4042,7 +4042,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="96926400"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4059,14 +4059,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="99" name="Picture 98" descr="223-wwe-320.png"/>
+        <xdr:cNvPr id="99" name="Picture 98" descr="RM-197.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4080,7 +4080,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="97936050"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4097,14 +4097,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>98</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="100" name="Picture 99" descr="223-wwe-321.png"/>
+        <xdr:cNvPr id="100" name="Picture 99" descr="RM-198.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4118,7 +4118,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="98945700"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4135,14 +4135,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>99</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="101" name="Picture 100" descr="223-wwe-322.png"/>
+        <xdr:cNvPr id="101" name="Picture 100" descr="RM-199.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4156,7 +4156,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="99955350"/>
-          <a:ext cx="2038350" cy="952500"/>
+          <a:ext cx="1419225" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>

<commit_message>
fix bugs open excel path from gui
</commit_message>
<xml_diff>
--- a/excel/barcode.xlsx
+++ b/excel/barcode.xlsx
@@ -16,304 +16,304 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
+    <t>RM-1</t>
+  </si>
+  <si>
+    <t>RM-2</t>
+  </si>
+  <si>
+    <t>RM-3</t>
+  </si>
+  <si>
+    <t>RM-4</t>
+  </si>
+  <si>
+    <t>RM-5</t>
+  </si>
+  <si>
+    <t>RM-6</t>
+  </si>
+  <si>
+    <t>RM-7</t>
+  </si>
+  <si>
+    <t>RM-8</t>
+  </si>
+  <si>
+    <t>RM-9</t>
+  </si>
+  <si>
+    <t>RM-10</t>
+  </si>
+  <si>
+    <t>RM-11</t>
+  </si>
+  <si>
+    <t>RM-12</t>
+  </si>
+  <si>
+    <t>RM-13</t>
+  </si>
+  <si>
+    <t>RM-14</t>
+  </si>
+  <si>
+    <t>RM-15</t>
+  </si>
+  <si>
+    <t>RM-16</t>
+  </si>
+  <si>
+    <t>RM-17</t>
+  </si>
+  <si>
+    <t>RM-18</t>
+  </si>
+  <si>
+    <t>RM-19</t>
+  </si>
+  <si>
+    <t>RM-20</t>
+  </si>
+  <si>
+    <t>RM-21</t>
+  </si>
+  <si>
+    <t>RM-22</t>
+  </si>
+  <si>
+    <t>RM-23</t>
+  </si>
+  <si>
+    <t>RM-24</t>
+  </si>
+  <si>
+    <t>RM-25</t>
+  </si>
+  <si>
+    <t>RM-26</t>
+  </si>
+  <si>
+    <t>RM-27</t>
+  </si>
+  <si>
+    <t>RM-28</t>
+  </si>
+  <si>
+    <t>RM-29</t>
+  </si>
+  <si>
+    <t>RM-30</t>
+  </si>
+  <si>
+    <t>RM-31</t>
+  </si>
+  <si>
+    <t>RM-32</t>
+  </si>
+  <si>
+    <t>RM-33</t>
+  </si>
+  <si>
+    <t>RM-34</t>
+  </si>
+  <si>
+    <t>RM-35</t>
+  </si>
+  <si>
+    <t>RM-36</t>
+  </si>
+  <si>
+    <t>RM-37</t>
+  </si>
+  <si>
+    <t>RM-38</t>
+  </si>
+  <si>
+    <t>RM-39</t>
+  </si>
+  <si>
+    <t>RM-40</t>
+  </si>
+  <si>
+    <t>RM-41</t>
+  </si>
+  <si>
+    <t>RM-42</t>
+  </si>
+  <si>
+    <t>RM-43</t>
+  </si>
+  <si>
+    <t>RM-44</t>
+  </si>
+  <si>
+    <t>RM-45</t>
+  </si>
+  <si>
+    <t>RM-46</t>
+  </si>
+  <si>
+    <t>RM-47</t>
+  </si>
+  <si>
+    <t>RM-48</t>
+  </si>
+  <si>
+    <t>RM-49</t>
+  </si>
+  <si>
+    <t>RM-50</t>
+  </si>
+  <si>
+    <t>RM-51</t>
+  </si>
+  <si>
+    <t>RM-52</t>
+  </si>
+  <si>
+    <t>RM-53</t>
+  </si>
+  <si>
+    <t>RM-54</t>
+  </si>
+  <si>
+    <t>RM-55</t>
+  </si>
+  <si>
+    <t>RM-56</t>
+  </si>
+  <si>
+    <t>RM-57</t>
+  </si>
+  <si>
+    <t>RM-58</t>
+  </si>
+  <si>
+    <t>RM-59</t>
+  </si>
+  <si>
+    <t>RM-60</t>
+  </si>
+  <si>
+    <t>RM-61</t>
+  </si>
+  <si>
+    <t>RM-62</t>
+  </si>
+  <si>
+    <t>RM-63</t>
+  </si>
+  <si>
+    <t>RM-64</t>
+  </si>
+  <si>
+    <t>RM-65</t>
+  </si>
+  <si>
+    <t>RM-66</t>
+  </si>
+  <si>
+    <t>RM-67</t>
+  </si>
+  <si>
+    <t>RM-68</t>
+  </si>
+  <si>
+    <t>RM-69</t>
+  </si>
+  <si>
+    <t>RM-70</t>
+  </si>
+  <si>
+    <t>RM-71</t>
+  </si>
+  <si>
+    <t>RM-72</t>
+  </si>
+  <si>
+    <t>RM-73</t>
+  </si>
+  <si>
+    <t>RM-74</t>
+  </si>
+  <si>
+    <t>RM-75</t>
+  </si>
+  <si>
+    <t>RM-76</t>
+  </si>
+  <si>
+    <t>RM-77</t>
+  </si>
+  <si>
+    <t>RM-78</t>
+  </si>
+  <si>
+    <t>RM-79</t>
+  </si>
+  <si>
+    <t>RM-80</t>
+  </si>
+  <si>
+    <t>RM-81</t>
+  </si>
+  <si>
+    <t>RM-82</t>
+  </si>
+  <si>
+    <t>RM-83</t>
+  </si>
+  <si>
+    <t>RM-84</t>
+  </si>
+  <si>
+    <t>RM-85</t>
+  </si>
+  <si>
+    <t>RM-86</t>
+  </si>
+  <si>
+    <t>RM-87</t>
+  </si>
+  <si>
+    <t>RM-88</t>
+  </si>
+  <si>
+    <t>RM-89</t>
+  </si>
+  <si>
+    <t>RM-90</t>
+  </si>
+  <si>
+    <t>RM-91</t>
+  </si>
+  <si>
+    <t>RM-92</t>
+  </si>
+  <si>
+    <t>RM-93</t>
+  </si>
+  <si>
+    <t>RM-94</t>
+  </si>
+  <si>
+    <t>RM-95</t>
+  </si>
+  <si>
+    <t>RM-96</t>
+  </si>
+  <si>
+    <t>RM-97</t>
+  </si>
+  <si>
+    <t>RM-98</t>
+  </si>
+  <si>
+    <t>RM-99</t>
+  </si>
+  <si>
     <t>RM-100</t>
-  </si>
-  <si>
-    <t>RM-101</t>
-  </si>
-  <si>
-    <t>RM-102</t>
-  </si>
-  <si>
-    <t>RM-103</t>
-  </si>
-  <si>
-    <t>RM-104</t>
-  </si>
-  <si>
-    <t>RM-105</t>
-  </si>
-  <si>
-    <t>RM-106</t>
-  </si>
-  <si>
-    <t>RM-107</t>
-  </si>
-  <si>
-    <t>RM-108</t>
-  </si>
-  <si>
-    <t>RM-109</t>
-  </si>
-  <si>
-    <t>RM-110</t>
-  </si>
-  <si>
-    <t>RM-111</t>
-  </si>
-  <si>
-    <t>RM-112</t>
-  </si>
-  <si>
-    <t>RM-113</t>
-  </si>
-  <si>
-    <t>RM-114</t>
-  </si>
-  <si>
-    <t>RM-115</t>
-  </si>
-  <si>
-    <t>RM-116</t>
-  </si>
-  <si>
-    <t>RM-117</t>
-  </si>
-  <si>
-    <t>RM-118</t>
-  </si>
-  <si>
-    <t>RM-119</t>
-  </si>
-  <si>
-    <t>RM-120</t>
-  </si>
-  <si>
-    <t>RM-121</t>
-  </si>
-  <si>
-    <t>RM-122</t>
-  </si>
-  <si>
-    <t>RM-123</t>
-  </si>
-  <si>
-    <t>RM-124</t>
-  </si>
-  <si>
-    <t>RM-125</t>
-  </si>
-  <si>
-    <t>RM-126</t>
-  </si>
-  <si>
-    <t>RM-127</t>
-  </si>
-  <si>
-    <t>RM-128</t>
-  </si>
-  <si>
-    <t>RM-129</t>
-  </si>
-  <si>
-    <t>RM-130</t>
-  </si>
-  <si>
-    <t>RM-131</t>
-  </si>
-  <si>
-    <t>RM-132</t>
-  </si>
-  <si>
-    <t>RM-133</t>
-  </si>
-  <si>
-    <t>RM-134</t>
-  </si>
-  <si>
-    <t>RM-135</t>
-  </si>
-  <si>
-    <t>RM-136</t>
-  </si>
-  <si>
-    <t>RM-137</t>
-  </si>
-  <si>
-    <t>RM-138</t>
-  </si>
-  <si>
-    <t>RM-139</t>
-  </si>
-  <si>
-    <t>RM-140</t>
-  </si>
-  <si>
-    <t>RM-141</t>
-  </si>
-  <si>
-    <t>RM-142</t>
-  </si>
-  <si>
-    <t>RM-143</t>
-  </si>
-  <si>
-    <t>RM-144</t>
-  </si>
-  <si>
-    <t>RM-145</t>
-  </si>
-  <si>
-    <t>RM-146</t>
-  </si>
-  <si>
-    <t>RM-147</t>
-  </si>
-  <si>
-    <t>RM-148</t>
-  </si>
-  <si>
-    <t>RM-149</t>
-  </si>
-  <si>
-    <t>RM-150</t>
-  </si>
-  <si>
-    <t>RM-151</t>
-  </si>
-  <si>
-    <t>RM-152</t>
-  </si>
-  <si>
-    <t>RM-153</t>
-  </si>
-  <si>
-    <t>RM-154</t>
-  </si>
-  <si>
-    <t>RM-155</t>
-  </si>
-  <si>
-    <t>RM-156</t>
-  </si>
-  <si>
-    <t>RM-157</t>
-  </si>
-  <si>
-    <t>RM-158</t>
-  </si>
-  <si>
-    <t>RM-159</t>
-  </si>
-  <si>
-    <t>RM-160</t>
-  </si>
-  <si>
-    <t>RM-161</t>
-  </si>
-  <si>
-    <t>RM-162</t>
-  </si>
-  <si>
-    <t>RM-163</t>
-  </si>
-  <si>
-    <t>RM-164</t>
-  </si>
-  <si>
-    <t>RM-165</t>
-  </si>
-  <si>
-    <t>RM-166</t>
-  </si>
-  <si>
-    <t>RM-167</t>
-  </si>
-  <si>
-    <t>RM-168</t>
-  </si>
-  <si>
-    <t>RM-169</t>
-  </si>
-  <si>
-    <t>RM-170</t>
-  </si>
-  <si>
-    <t>RM-171</t>
-  </si>
-  <si>
-    <t>RM-172</t>
-  </si>
-  <si>
-    <t>RM-173</t>
-  </si>
-  <si>
-    <t>RM-174</t>
-  </si>
-  <si>
-    <t>RM-175</t>
-  </si>
-  <si>
-    <t>RM-176</t>
-  </si>
-  <si>
-    <t>RM-177</t>
-  </si>
-  <si>
-    <t>RM-178</t>
-  </si>
-  <si>
-    <t>RM-179</t>
-  </si>
-  <si>
-    <t>RM-180</t>
-  </si>
-  <si>
-    <t>RM-181</t>
-  </si>
-  <si>
-    <t>RM-182</t>
-  </si>
-  <si>
-    <t>RM-183</t>
-  </si>
-  <si>
-    <t>RM-184</t>
-  </si>
-  <si>
-    <t>RM-185</t>
-  </si>
-  <si>
-    <t>RM-186</t>
-  </si>
-  <si>
-    <t>RM-187</t>
-  </si>
-  <si>
-    <t>RM-188</t>
-  </si>
-  <si>
-    <t>RM-189</t>
-  </si>
-  <si>
-    <t>RM-190</t>
-  </si>
-  <si>
-    <t>RM-191</t>
-  </si>
-  <si>
-    <t>RM-192</t>
-  </si>
-  <si>
-    <t>RM-193</t>
-  </si>
-  <si>
-    <t>RM-194</t>
-  </si>
-  <si>
-    <t>RM-195</t>
-  </si>
-  <si>
-    <t>RM-196</t>
-  </si>
-  <si>
-    <t>RM-197</t>
-  </si>
-  <si>
-    <t>RM-198</t>
-  </si>
-  <si>
-    <t>RM-199</t>
   </si>
 </sst>
 </file>
@@ -373,14 +373,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="RM-100.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="RM-1.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -394,7 +394,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="0"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1171575" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -411,14 +411,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="RM-101.png"/>
+        <xdr:cNvPr id="3" name="Picture 2" descr="RM-2.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -432,7 +432,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="1009650"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1171575" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -449,14 +449,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="RM-102.png"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="RM-3.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -470,7 +470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="2019300"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1171575" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -487,14 +487,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="RM-103.png"/>
+        <xdr:cNvPr id="5" name="Picture 4" descr="RM-4.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -508,7 +508,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="3028950"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1171575" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -525,14 +525,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="RM-104.png"/>
+        <xdr:cNvPr id="6" name="Picture 5" descr="RM-5.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -546,7 +546,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="4038600"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1171575" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -563,14 +563,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="RM-105.png"/>
+        <xdr:cNvPr id="7" name="Picture 6" descr="RM-6.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -584,7 +584,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="5048250"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1171575" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -601,14 +601,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="RM-106.png"/>
+        <xdr:cNvPr id="8" name="Picture 7" descr="RM-7.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -622,7 +622,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="6057900"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1171575" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -639,14 +639,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="RM-107.png"/>
+        <xdr:cNvPr id="9" name="Picture 8" descr="RM-8.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -660,7 +660,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="7067550"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1171575" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -677,14 +677,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="RM-108.png"/>
+        <xdr:cNvPr id="10" name="Picture 9" descr="RM-9.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -698,7 +698,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="8077200"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1171575" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -716,13 +716,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="RM-109.png"/>
+        <xdr:cNvPr id="11" name="Picture 10" descr="RM-10.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -736,7 +736,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="9086850"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -754,13 +754,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="RM-110.png"/>
+        <xdr:cNvPr id="12" name="Picture 11" descr="RM-11.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -774,7 +774,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="10096500"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -792,13 +792,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="RM-111.png"/>
+        <xdr:cNvPr id="13" name="Picture 12" descr="RM-12.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -812,7 +812,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="11106150"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -830,13 +830,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="RM-112.png"/>
+        <xdr:cNvPr id="14" name="Picture 13" descr="RM-13.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -850,7 +850,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="12115800"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -868,13 +868,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14" descr="RM-113.png"/>
+        <xdr:cNvPr id="15" name="Picture 14" descr="RM-14.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -888,7 +888,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="13125450"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -906,13 +906,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15" descr="RM-114.png"/>
+        <xdr:cNvPr id="16" name="Picture 15" descr="RM-15.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -926,7 +926,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="14135100"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -944,13 +944,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16" descr="RM-115.png"/>
+        <xdr:cNvPr id="17" name="Picture 16" descr="RM-16.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -964,7 +964,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="15144750"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -982,13 +982,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17" descr="RM-116.png"/>
+        <xdr:cNvPr id="18" name="Picture 17" descr="RM-17.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1002,7 +1002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="16154400"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1020,13 +1020,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18" descr="RM-117.png"/>
+        <xdr:cNvPr id="19" name="Picture 18" descr="RM-18.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1040,7 +1040,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="17164050"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1058,13 +1058,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19" descr="RM-118.png"/>
+        <xdr:cNvPr id="20" name="Picture 19" descr="RM-19.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1078,7 +1078,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="18173700"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1096,13 +1096,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20" descr="RM-119.png"/>
+        <xdr:cNvPr id="21" name="Picture 20" descr="RM-20.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1116,7 +1116,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="19183350"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1134,13 +1134,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21" descr="RM-120.png"/>
+        <xdr:cNvPr id="22" name="Picture 21" descr="RM-21.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1154,7 +1154,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="20193000"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1172,13 +1172,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 22" descr="RM-121.png"/>
+        <xdr:cNvPr id="23" name="Picture 22" descr="RM-22.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1192,7 +1192,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="21202650"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1210,13 +1210,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23" descr="RM-122.png"/>
+        <xdr:cNvPr id="24" name="Picture 23" descr="RM-23.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1230,7 +1230,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="22212300"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1248,13 +1248,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24" descr="RM-123.png"/>
+        <xdr:cNvPr id="25" name="Picture 24" descr="RM-24.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1268,7 +1268,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="23221950"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1286,13 +1286,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Picture 25" descr="RM-124.png"/>
+        <xdr:cNvPr id="26" name="Picture 25" descr="RM-25.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1306,7 +1306,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="24231600"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1324,13 +1324,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="27" name="Picture 26" descr="RM-125.png"/>
+        <xdr:cNvPr id="27" name="Picture 26" descr="RM-26.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1344,7 +1344,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="25241250"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1362,13 +1362,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Picture 27" descr="RM-126.png"/>
+        <xdr:cNvPr id="28" name="Picture 27" descr="RM-27.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1382,7 +1382,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="26250900"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1400,13 +1400,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="Picture 28" descr="RM-127.png"/>
+        <xdr:cNvPr id="29" name="Picture 28" descr="RM-28.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1420,7 +1420,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="27260550"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1438,13 +1438,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Picture 29" descr="RM-128.png"/>
+        <xdr:cNvPr id="30" name="Picture 29" descr="RM-29.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1458,7 +1458,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="28270200"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1476,13 +1476,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="Picture 30" descr="RM-129.png"/>
+        <xdr:cNvPr id="31" name="Picture 30" descr="RM-30.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1496,7 +1496,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="29279850"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1514,13 +1514,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="32" name="Picture 31" descr="RM-130.png"/>
+        <xdr:cNvPr id="32" name="Picture 31" descr="RM-31.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1534,7 +1534,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="30289500"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1552,13 +1552,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Picture 32" descr="RM-131.png"/>
+        <xdr:cNvPr id="33" name="Picture 32" descr="RM-32.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1572,7 +1572,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="31299150"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1590,13 +1590,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Picture 33" descr="RM-132.png"/>
+        <xdr:cNvPr id="34" name="Picture 33" descr="RM-33.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1610,7 +1610,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="32308800"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1628,13 +1628,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Picture 34" descr="RM-133.png"/>
+        <xdr:cNvPr id="35" name="Picture 34" descr="RM-34.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1648,7 +1648,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="33318450"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1666,13 +1666,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="Picture 35" descr="RM-134.png"/>
+        <xdr:cNvPr id="36" name="Picture 35" descr="RM-35.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1686,7 +1686,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="34328100"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1704,13 +1704,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Picture 36" descr="RM-135.png"/>
+        <xdr:cNvPr id="37" name="Picture 36" descr="RM-36.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1724,7 +1724,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="35337750"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1742,13 +1742,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 37" descr="RM-136.png"/>
+        <xdr:cNvPr id="38" name="Picture 37" descr="RM-37.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1762,7 +1762,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="36347400"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1780,13 +1780,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Picture 38" descr="RM-137.png"/>
+        <xdr:cNvPr id="39" name="Picture 38" descr="RM-38.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1800,7 +1800,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="37357050"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1818,13 +1818,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="Picture 39" descr="RM-138.png"/>
+        <xdr:cNvPr id="40" name="Picture 39" descr="RM-39.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1838,7 +1838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="38366700"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1856,13 +1856,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Picture 40" descr="RM-139.png"/>
+        <xdr:cNvPr id="41" name="Picture 40" descr="RM-40.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1876,7 +1876,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="39376350"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1894,13 +1894,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="Picture 41" descr="RM-140.png"/>
+        <xdr:cNvPr id="42" name="Picture 41" descr="RM-41.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1914,7 +1914,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="40386000"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1932,13 +1932,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="Picture 42" descr="RM-141.png"/>
+        <xdr:cNvPr id="43" name="Picture 42" descr="RM-42.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1952,7 +1952,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="41395650"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1970,13 +1970,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="44" name="Picture 43" descr="RM-142.png"/>
+        <xdr:cNvPr id="44" name="Picture 43" descr="RM-43.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1990,7 +1990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="42405300"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2008,13 +2008,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="45" name="Picture 44" descr="RM-143.png"/>
+        <xdr:cNvPr id="45" name="Picture 44" descr="RM-44.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2028,7 +2028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="43414950"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2046,13 +2046,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="46" name="Picture 45" descr="RM-144.png"/>
+        <xdr:cNvPr id="46" name="Picture 45" descr="RM-45.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2066,7 +2066,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="44424600"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2084,13 +2084,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="Picture 46" descr="RM-145.png"/>
+        <xdr:cNvPr id="47" name="Picture 46" descr="RM-46.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2104,7 +2104,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="45434250"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2122,13 +2122,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="48" name="Picture 47" descr="RM-146.png"/>
+        <xdr:cNvPr id="48" name="Picture 47" descr="RM-47.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2142,7 +2142,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="46443900"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2160,13 +2160,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="49" name="Picture 48" descr="RM-147.png"/>
+        <xdr:cNvPr id="49" name="Picture 48" descr="RM-48.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2180,7 +2180,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="47453550"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2198,13 +2198,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="50" name="Picture 49" descr="RM-148.png"/>
+        <xdr:cNvPr id="50" name="Picture 49" descr="RM-49.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2218,7 +2218,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="48463200"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2236,13 +2236,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="51" name="Picture 50" descr="RM-149.png"/>
+        <xdr:cNvPr id="51" name="Picture 50" descr="RM-50.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2256,7 +2256,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="49472850"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2274,13 +2274,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="52" name="Picture 51" descr="RM-150.png"/>
+        <xdr:cNvPr id="52" name="Picture 51" descr="RM-51.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2294,7 +2294,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="50482500"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2312,13 +2312,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="53" name="Picture 52" descr="RM-151.png"/>
+        <xdr:cNvPr id="53" name="Picture 52" descr="RM-52.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2332,7 +2332,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="51492150"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2350,13 +2350,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="54" name="Picture 53" descr="RM-152.png"/>
+        <xdr:cNvPr id="54" name="Picture 53" descr="RM-53.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2370,7 +2370,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="52501800"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2388,13 +2388,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="Picture 54" descr="RM-153.png"/>
+        <xdr:cNvPr id="55" name="Picture 54" descr="RM-54.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2408,7 +2408,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="53511450"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2426,13 +2426,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="56" name="Picture 55" descr="RM-154.png"/>
+        <xdr:cNvPr id="56" name="Picture 55" descr="RM-55.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2446,7 +2446,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="54521100"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2464,13 +2464,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="57" name="Picture 56" descr="RM-155.png"/>
+        <xdr:cNvPr id="57" name="Picture 56" descr="RM-56.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2484,7 +2484,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="55530750"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2502,13 +2502,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="58" name="Picture 57" descr="RM-156.png"/>
+        <xdr:cNvPr id="58" name="Picture 57" descr="RM-57.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2522,7 +2522,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="56540400"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2540,13 +2540,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="59" name="Picture 58" descr="RM-157.png"/>
+        <xdr:cNvPr id="59" name="Picture 58" descr="RM-58.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2560,7 +2560,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="57550050"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2578,13 +2578,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="60" name="Picture 59" descr="RM-158.png"/>
+        <xdr:cNvPr id="60" name="Picture 59" descr="RM-59.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2598,7 +2598,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="58559700"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2616,13 +2616,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>59</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61" name="Picture 60" descr="RM-159.png"/>
+        <xdr:cNvPr id="61" name="Picture 60" descr="RM-60.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2636,7 +2636,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="59569350"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2654,13 +2654,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="62" name="Picture 61" descr="RM-160.png"/>
+        <xdr:cNvPr id="62" name="Picture 61" descr="RM-61.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2674,7 +2674,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="60579000"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2692,13 +2692,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="63" name="Picture 62" descr="RM-161.png"/>
+        <xdr:cNvPr id="63" name="Picture 62" descr="RM-62.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2712,7 +2712,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="61588650"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2730,13 +2730,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="64" name="Picture 63" descr="RM-162.png"/>
+        <xdr:cNvPr id="64" name="Picture 63" descr="RM-63.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2750,7 +2750,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="62598300"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2768,13 +2768,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="65" name="Picture 64" descr="RM-163.png"/>
+        <xdr:cNvPr id="65" name="Picture 64" descr="RM-64.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2788,7 +2788,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="63607950"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2806,13 +2806,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="66" name="Picture 65" descr="RM-164.png"/>
+        <xdr:cNvPr id="66" name="Picture 65" descr="RM-65.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2826,7 +2826,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="64617600"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2844,13 +2844,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="67" name="Picture 66" descr="RM-165.png"/>
+        <xdr:cNvPr id="67" name="Picture 66" descr="RM-66.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2864,7 +2864,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="65627250"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2882,13 +2882,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="68" name="Picture 67" descr="RM-166.png"/>
+        <xdr:cNvPr id="68" name="Picture 67" descr="RM-67.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2902,7 +2902,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="66636900"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2920,13 +2920,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="69" name="Picture 68" descr="RM-167.png"/>
+        <xdr:cNvPr id="69" name="Picture 68" descr="RM-68.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2940,7 +2940,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="67646550"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2958,13 +2958,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="Picture 69" descr="RM-168.png"/>
+        <xdr:cNvPr id="70" name="Picture 69" descr="RM-69.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2978,7 +2978,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="68656200"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2996,13 +2996,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="71" name="Picture 70" descr="RM-169.png"/>
+        <xdr:cNvPr id="71" name="Picture 70" descr="RM-70.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3016,7 +3016,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="69665850"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3034,13 +3034,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="72" name="Picture 71" descr="RM-170.png"/>
+        <xdr:cNvPr id="72" name="Picture 71" descr="RM-71.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3054,7 +3054,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="70675500"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3072,13 +3072,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>71</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="73" name="Picture 72" descr="RM-171.png"/>
+        <xdr:cNvPr id="73" name="Picture 72" descr="RM-72.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3092,7 +3092,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="71685150"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3110,13 +3110,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="74" name="Picture 73" descr="RM-172.png"/>
+        <xdr:cNvPr id="74" name="Picture 73" descr="RM-73.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3130,7 +3130,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="72694800"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3148,13 +3148,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="75" name="Picture 74" descr="RM-173.png"/>
+        <xdr:cNvPr id="75" name="Picture 74" descr="RM-74.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3168,7 +3168,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="73704450"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3186,13 +3186,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>74</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="76" name="Picture 75" descr="RM-174.png"/>
+        <xdr:cNvPr id="76" name="Picture 75" descr="RM-75.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3206,7 +3206,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="74714100"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3224,13 +3224,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="77" name="Picture 76" descr="RM-175.png"/>
+        <xdr:cNvPr id="77" name="Picture 76" descr="RM-76.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3244,7 +3244,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="75723750"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3262,13 +3262,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="78" name="Picture 77" descr="RM-176.png"/>
+        <xdr:cNvPr id="78" name="Picture 77" descr="RM-77.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3282,7 +3282,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="76733400"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3300,13 +3300,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>77</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="79" name="Picture 78" descr="RM-177.png"/>
+        <xdr:cNvPr id="79" name="Picture 78" descr="RM-78.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3320,7 +3320,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="77743050"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3338,13 +3338,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="80" name="Picture 79" descr="RM-178.png"/>
+        <xdr:cNvPr id="80" name="Picture 79" descr="RM-79.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3358,7 +3358,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="78752700"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3376,13 +3376,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>79</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="81" name="Picture 80" descr="RM-179.png"/>
+        <xdr:cNvPr id="81" name="Picture 80" descr="RM-80.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3396,7 +3396,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="79762350"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3414,13 +3414,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>80</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="82" name="Picture 81" descr="RM-180.png"/>
+        <xdr:cNvPr id="82" name="Picture 81" descr="RM-81.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3434,7 +3434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="80772000"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3452,13 +3452,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="83" name="Picture 82" descr="RM-181.png"/>
+        <xdr:cNvPr id="83" name="Picture 82" descr="RM-82.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3472,7 +3472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="81781650"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3490,13 +3490,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>82</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="84" name="Picture 83" descr="RM-182.png"/>
+        <xdr:cNvPr id="84" name="Picture 83" descr="RM-83.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3510,7 +3510,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="82791300"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3528,13 +3528,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="85" name="Picture 84" descr="RM-183.png"/>
+        <xdr:cNvPr id="85" name="Picture 84" descr="RM-84.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3548,7 +3548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="83800950"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3566,13 +3566,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>84</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="86" name="Picture 85" descr="RM-184.png"/>
+        <xdr:cNvPr id="86" name="Picture 85" descr="RM-85.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3586,7 +3586,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="84810600"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3604,13 +3604,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>85</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="87" name="Picture 86" descr="RM-185.png"/>
+        <xdr:cNvPr id="87" name="Picture 86" descr="RM-86.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3624,7 +3624,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="85820250"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3642,13 +3642,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>86</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="88" name="Picture 87" descr="RM-186.png"/>
+        <xdr:cNvPr id="88" name="Picture 87" descr="RM-87.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3662,7 +3662,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="86829900"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3680,13 +3680,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>87</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="89" name="Picture 88" descr="RM-187.png"/>
+        <xdr:cNvPr id="89" name="Picture 88" descr="RM-88.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3700,7 +3700,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="87839550"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3718,13 +3718,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="90" name="Picture 89" descr="RM-188.png"/>
+        <xdr:cNvPr id="90" name="Picture 89" descr="RM-89.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3738,7 +3738,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="88849200"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3756,13 +3756,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>89</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="91" name="Picture 90" descr="RM-189.png"/>
+        <xdr:cNvPr id="91" name="Picture 90" descr="RM-90.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3776,7 +3776,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="89858850"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3794,13 +3794,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>90</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="92" name="Picture 91" descr="RM-190.png"/>
+        <xdr:cNvPr id="92" name="Picture 91" descr="RM-91.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3814,7 +3814,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="90868500"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3832,13 +3832,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>91</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="93" name="Picture 92" descr="RM-191.png"/>
+        <xdr:cNvPr id="93" name="Picture 92" descr="RM-92.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3852,7 +3852,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="91878150"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3870,13 +3870,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>92</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="94" name="Picture 93" descr="RM-192.png"/>
+        <xdr:cNvPr id="94" name="Picture 93" descr="RM-93.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3890,7 +3890,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="92887800"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3908,13 +3908,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>93</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="95" name="Picture 94" descr="RM-193.png"/>
+        <xdr:cNvPr id="95" name="Picture 94" descr="RM-94.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3928,7 +3928,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="93897450"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3946,13 +3946,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>94</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="96" name="Picture 95" descr="RM-194.png"/>
+        <xdr:cNvPr id="96" name="Picture 95" descr="RM-95.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3966,7 +3966,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="94907100"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3984,13 +3984,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="97" name="Picture 96" descr="RM-195.png"/>
+        <xdr:cNvPr id="97" name="Picture 96" descr="RM-96.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4004,7 +4004,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="95916750"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4022,13 +4022,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>96</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="98" name="Picture 97" descr="RM-196.png"/>
+        <xdr:cNvPr id="98" name="Picture 97" descr="RM-97.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4042,7 +4042,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="96926400"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4060,13 +4060,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>97</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="99" name="Picture 98" descr="RM-197.png"/>
+        <xdr:cNvPr id="99" name="Picture 98" descr="RM-98.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4080,7 +4080,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="97936050"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4098,13 +4098,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>98</xdr:row>
       <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="100" name="Picture 99" descr="RM-198.png"/>
+        <xdr:cNvPr id="100" name="Picture 99" descr="RM-99.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4118,7 +4118,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2047875" y="98945700"/>
-          <a:ext cx="1419225" cy="952500"/>
+          <a:ext cx="1295400" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4142,7 +4142,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="101" name="Picture 100" descr="RM-199.png"/>
+        <xdr:cNvPr id="101" name="Picture 100" descr="RM-100.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>